<commit_message>
bersihin yg ga kepake
</commit_message>
<xml_diff>
--- a/predicted_answers.xlsx
+++ b/predicted_answers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,19 +460,19 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ajshdkjahsjkdasd'</t>
+          <t>asiap ah</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dajshdjkajksdhjkasjkdhqiwuehqweqwe</t>
+          <t>acid</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,19 +484,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>acid</t>
+          <t>sql</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ai</t>
+          <t>nosql</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,12 +508,132 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ngaco</t>
+          <t>normalization</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>data mining</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>buset dah</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>chatbot</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>apa itu chatbot</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>vr</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>iot</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>djkashdjkjahsdlalshdlkasd</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>aasaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>siem</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>metadata</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
latih model dan testing
</commit_message>
<xml_diff>
--- a/predicted_answers.xlsx
+++ b/predicted_answers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>go</t>
+          <t>api?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>asiap ah</t>
+          <t>oop</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>acid</t>
+          <t>asiap</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,31 +484,31 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sql</t>
+          <t>commit dalam git?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>nosql</t>
+          <t>bahasa pemrograman tingkat rendah</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>normalization</t>
+          <t>debungging</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>data mining</t>
+          <t>apa itu go</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>buset dah</t>
+          <t>ai</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>chatbot</t>
+          <t>ai</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>apa itu chatbot</t>
+          <t>ai</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>vr</t>
+          <t>ai</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,19 +580,19 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>iot</t>
+          <t>acid</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>djkashdjkjahsdlalshdlkasd</t>
+          <t>debungging</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,36 +604,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>aasaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+          <t>commit dalam git?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>siem</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>metadata</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
testing dan hasil dari testing
</commit_message>
<xml_diff>
--- a/predicted_answers.xlsx
+++ b/predicted_answers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,43 +448,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>api?</t>
+          <t>go</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>oop</t>
+          <t>ai</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>asiap</t>
+          <t>acid</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
+          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>commit dalam git?</t>
+          <t>apa itu acid</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>bahasa pemrograman tingkat rendah</t>
+          <t>apa itu ai</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,106 +508,10 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>debungging</t>
+          <t xml:space="preserve">exit </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>apa itu go</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ai</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ai</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ai</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>ai</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>acid</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>debungging</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ACID adalah sekumpulan properti (Atomicity, Consistency, Isolation, Durability) yang menjamin keandalan transaksi dalam basis data.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>commit dalam git?</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
         <is>
           <t>AI adalah Artificial Intelligence, yaitu kecerdasan buatan yang memungkinkan mesin untuk meniru kecerdasan manusia dalam menyelesaikan tugas.</t>
         </is>

</xml_diff>